<commit_message>
DN node 9. RES updated
</commit_message>
<xml_diff>
--- a/data/IEEE9/ieee18_2/ieee18_2_2035.xlsx
+++ b/data/IEEE9/ieee18_2/ieee18_2_2035.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\thesis-shared-resources-planning-no_esso-degradation\data\IEEE9\ieee18_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE0B59B3-FFC9-4A71-A125-309CC8D4925A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67521466-C53B-4ADE-84FF-CBB0BBF21573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="4560" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8355" yWindow="4620" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -13486,11 +13486,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.587773224043715E-5</v>
+        <v>4.4515027322404366E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5611837493523512E-5</v>
+        <v>2.4827801651885036E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13510,15 +13510,15 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0697222114439296E-2</v>
+        <v>4.4088657290642583E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.90939518785677864</v>
+        <v>0.83144702889762612</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2235023052025991</v>
+        <v>2.1176212430500945</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13526,23 +13526,23 @@
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2249943118916242</v>
+        <v>3.1617591293055138</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2155450274371282</v>
+        <v>3.1492451299641977</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8861614187654476</v>
+        <v>2.7707149620148295</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2152205596220442</v>
+        <v>2.3294071864066859</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.275796715394713</v>
+        <v>1.2386375877618574</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13550,15 +13550,15 @@
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8284070407040731E-3</v>
+        <v>1.7756645299145325E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9416751978919505E-4</v>
+        <v>3.1868147977162799E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.3227804699643408E-5</v>
+        <v>7.918762000548597E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13583,99 +13583,99 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1498235461016248</v>
+        <v>2.9357578682112226</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7521552126607762</v>
+        <v>2.6965561174555082</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.864972978188693</v>
+        <v>2.7012602365779106</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7074410111066287</v>
+        <v>2.6253973441033973</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2499070939836967</v>
+        <v>2.3920064893931934</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0903071551036558</v>
+        <v>2.1530163697567657</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8002359356040025</v>
+        <v>1.855345198938819</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5998415811224072</v>
+        <v>1.6658144298284858</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5824703422091801</v>
+        <v>1.5663226856560251</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5188478698763828</v>
+        <v>1.400879103284042</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4353895823832163</v>
+        <v>1.4788862363948292</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3725347153462339</v>
+        <v>1.4736688522664827</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3257307195545065</v>
+        <v>1.4204257709512569</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.266301334361758</v>
+        <v>1.2796308220918817</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6117382592434768</v>
+        <v>1.7460497808471001</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.86881125351375</v>
+        <v>1.8127469159083374</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.031179519378032</v>
+        <v>1.8749349409643368</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.205121327278559</v>
+        <v>2.1186459811107721</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9527976069330966</v>
+        <v>2.0966879569176409</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2084099750182382</v>
+        <v>2.0611826433503557</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1683292203553566</v>
+        <v>2.1240776036134101</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3839255580606258</v>
+        <v>2.3158133992588938</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3069530910473475</v>
+        <v>2.1751272001303561</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5573650008493503</v>
+        <v>2.4332210687692846</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -13688,11 +13688,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7260928961748631E-5</v>
+        <v>1.7987704918032785E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0349273109627868E-5</v>
+        <v>1.0035658772972477E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13712,31 +13712,31 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6448460604585883E-2</v>
+        <v>1.6109317086965558E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33950753679986401</v>
+        <v>0.36375807514271147</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86398946716443847</v>
+        <v>0.84704849722003772</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1347425811255609</v>
+        <v>1.0893528778805384</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2520566152049835</v>
+        <v>1.2899977247566496</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3790378674369541</v>
+        <v>1.3525179084477819</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2121877958814882</v>
+        <v>1.2006431502064263</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13744,11 +13744,11 @@
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5004095854557904</v>
+        <v>0.49545503510474292</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11480140278105208</v>
+        <v>0.1137080560878992</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13756,11 +13756,11 @@
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2256979991216461E-4</v>
+        <v>1.2011840391392132E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2321477553259576E-5</v>
+        <v>3.2967907104324765E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13789,7 +13789,7 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8714480874316939E-5</v>
+        <v>1.8532786885245898E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13813,55 +13813,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7465891157446869E-2</v>
+        <v>1.6618032363396047E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36029371252230469</v>
+        <v>0.34643626204067757</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82163704230343659</v>
+        <v>0.87245995213663885</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1574374327480721</v>
+        <v>1.1687848585593277</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2014684691360951</v>
+        <v>1.2394095786877612</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3657778879423679</v>
+        <v>1.2596980519856791</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1890985045313645</v>
+        <v>1.2121877958814882</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.95003273484821704</v>
+        <v>0.86781836356327502</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.49050048475369551</v>
+        <v>0.48059138405160062</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.1137080560878992</v>
+        <v>0.10496128254267618</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.962011424219356E-4</v>
+        <v>6.8916880764999678E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2011840391392132E-4</v>
+        <v>1.2256979991216461E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1351833226661785E-5</v>
+        <v>3.1028618451129191E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13890,11 +13890,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7260928961748631E-5</v>
+        <v>1.8351092896174861E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.931120660754014E-6</v>
+        <v>1.0349273109627868E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13914,43 +13914,43 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6448460604585883E-2</v>
+        <v>1.6109317086965558E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35682934990189791</v>
+        <v>0.33604317417945723</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.8555189821922381</v>
+        <v>0.86398946716443847</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1460900069368165</v>
+        <v>1.0780054520692828</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2267625421705393</v>
+        <v>1.3152917977910936</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3127379699640236</v>
+        <v>1.2596980519856791</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1429199218311172</v>
+        <v>1.1198306304809937</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.87695329370604636</v>
+        <v>0.95003273484821704</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.5004095854557904</v>
+        <v>0.49545503510474292</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10605462923582906</v>
+        <v>0.11152136270159345</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -13958,11 +13958,11 @@
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1644130991655637E-4</v>
+        <v>1.2502119591040791E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0705403675596596E-5</v>
+        <v>3.1998262777726981E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14160,7 +14160,7 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.3606557377049174E-5</v>
+        <v>4.5423497267759557E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14188,51 +14188,51 @@
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.857429748550677</v>
+        <v>0.8920733747547448</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0117401808975894</v>
+        <v>2.2023260927720982</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7801193237576243</v>
+        <v>2.6950136301732068</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0036711728402379</v>
+        <v>3.098523946719403</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3812947711194545</v>
+        <v>3.3481448223829888</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.828438190390139</v>
+        <v>2.9727462613284112</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2380578849789727</v>
+        <v>2.3294071864066859</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.275796715394713</v>
+        <v>1.251023963639476</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.26240320635669045</v>
+        <v>0.2596698396238083</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8284070407040731E-3</v>
+        <v>1.7229220191249919E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0029600978480331E-4</v>
+        <v>3.0948874477821568E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4843878577306394E-5</v>
+        <v>8.3227804699643408E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14257,15 +14257,15 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2109851683560251</v>
+        <v>3.058081112720024</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8633534030713133</v>
+        <v>2.7799547602634105</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7285456935130408</v>
+        <v>2.7012602365779106</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14273,27 +14273,27 @@
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4630561870979415</v>
+        <v>2.4867394196661912</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1739194413078025</v>
+        <v>2.0066948688995097</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8737149533837578</v>
+        <v>1.8186056900489413</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5833483689458874</v>
+        <v>1.5998415811224072</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5340273725497153</v>
+        <v>1.5663226856560251</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5188478698763828</v>
+        <v>1.4746095824042549</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14301,35 +14301,35 @@
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4447733845749831</v>
+        <v>1.5025643199579823</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3798421774955067</v>
+        <v>1.4204257709512569</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3596077484726243</v>
+        <v>1.266301334361758</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7460497808471001</v>
+        <v>1.6117382592434768</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8127469159083374</v>
+        <v>1.8501231409786123</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0507100916797434</v>
+        <v>1.9335266578694723</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0754083080268786</v>
+        <v>2.205121327278559</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9527976069330966</v>
+        <v>2.1583552497681597</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14341,15 +14341,15 @@
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3839255580606258</v>
+        <v>2.3385174521928045</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1311852364913588</v>
+        <v>2.2190691637693529</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.383563495937258</v>
+        <v>2.5325362144333368</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -14362,11 +14362,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8714480874316939E-5</v>
+        <v>1.7806010928961748E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0244734997409405E-5</v>
+        <v>1.0035658772972477E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14386,55 +14386,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6278888845775719E-2</v>
+        <v>1.6618032363396047E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.34990062466108435</v>
+        <v>0.35336498728149113</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83857801224783735</v>
+        <v>0.81316655733123622</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1801322843705835</v>
+        <v>1.1347425811255609</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2141155056533173</v>
+        <v>1.2394095786877612</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3922978469315401</v>
+        <v>1.3790378674369541</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2121877958814882</v>
+        <v>1.09674133913087</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.89522315399158903</v>
+        <v>0.93176287456267437</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47068228334950574</v>
+        <v>0.51031868615788523</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10933466931528769</v>
+        <v>0.10386793584952331</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3839515105356807E-4</v>
+        <v>6.6807180333418054E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1766700791567802E-4</v>
+        <v>1.1889270591479966E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3291121879857366E-5</v>
+        <v>3.2321477553259576E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14463,11 +14463,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7624316939890707E-5</v>
+        <v>1.7442622950819669E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0453811221846331E-5</v>
+        <v>1.0767425558501721E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14487,15 +14487,15 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6448460604585883E-2</v>
+        <v>1.7635462916257033E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33950753679986401</v>
+        <v>0.35682934990189791</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.83010752727563697</v>
+        <v>0.81316655733123622</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14503,11 +14503,11 @@
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3026447612738716</v>
+        <v>1.2394095786877612</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2729580314802651</v>
+        <v>1.2862180109748513</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14515,19 +14515,19 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.87695329370604636</v>
+        <v>0.93176287456267437</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51031868615788523</v>
+        <v>0.49545503510474292</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11480140278105208</v>
+        <v>0.11152136270159345</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3839515105356807E-4</v>
+        <v>7.2433048150969054E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14535,7 +14535,7 @@
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2321477553259576E-5</v>
+        <v>3.1351833226661785E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14564,7 +14564,7 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7806010928961748E-5</v>
+        <v>1.7442622950819669E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14588,43 +14588,43 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7805034675067194E-2</v>
+        <v>1.6787604122206212E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35682934990189791</v>
+        <v>0.32911444893864367</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86398946716443847</v>
+        <v>0.80469607235903584</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1801322843705835</v>
+        <v>1.1347425811255609</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2394095786877612</v>
+        <v>1.3152917977910936</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3392579289531956</v>
+        <v>1.3259979494586096</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1082859848059319</v>
+        <v>1.1544645675061791</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94089780470544571</v>
+        <v>0.9134930142771317</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.48059138405160062</v>
+        <v>0.5004095854557904</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10605462923582906</v>
+        <v>0.10496128254267618</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14636,7 +14636,7 @@
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2321477553259576E-5</v>
+        <v>3.1675048002194387E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14834,11 +14834,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.587773224043715E-5</v>
+        <v>4.4060792349726766E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6657218615708143E-5</v>
+        <v>2.4827801651885036E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14858,39 +14858,39 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1969010305515531E-2</v>
+        <v>4.0697222114439296E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82278612234660919</v>
+        <v>0.84876884199965996</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0540926057585915</v>
+        <v>2.0752688181890924</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7233821947013457</v>
+        <v>2.9786992754545976</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1617591293055138</v>
+        <v>3.2249943118916242</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2818449249100592</v>
+        <v>3.1823950787006625</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.0016078755160658</v>
+        <v>2.828438190390139</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3522445117636144</v>
+        <v>2.3750818371205424</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3005694671499501</v>
+        <v>1.1767057083737644</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14898,15 +14898,15 @@
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7756645299145325E-3</v>
+        <v>1.7405028560548391E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.9110327479139094E-4</v>
+        <v>3.1255298977601978E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.7571546127822971E-5</v>
+        <v>7.918762000548597E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -14931,55 +14931,55 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1192427349744243</v>
+        <v>3.058081112720024</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.6409570222502401</v>
+        <v>2.6687565698528743</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7558311504481714</v>
+        <v>2.8104020643184322</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8168325671109375</v>
+        <v>2.8441804561120145</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.4156897219614426</v>
+        <v>2.2972735591201952</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0066948688995097</v>
+        <v>2.1112102266546926</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8186056900489413</v>
+        <v>1.8369754444938802</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6988008541815254</v>
+        <v>1.7317872785345645</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6793562815281096</v>
+        <v>1.598617998762335</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5483400615244678</v>
+        <v>1.5335939657004252</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5078840057359042</v>
+        <v>1.4643873517242918</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4158779168834834</v>
+        <v>1.4447733845749831</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4204257709512569</v>
+        <v>1.3122028550692564</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -14991,31 +14991,31 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9248755911191626</v>
+        <v>1.8501231409786123</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9335266578694723</v>
+        <v>1.8554043686626251</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0970271445688256</v>
+        <v>2.0537894714849321</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9939091355001093</v>
+        <v>2.1583552497681597</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.103247595255465</v>
+        <v>2.1453125471605743</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3232098789521678</v>
+        <v>2.1904550287263294</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2704052933910721</v>
+        <v>2.2249971875232504</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -15023,7 +15023,7 @@
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.5077074280173237</v>
+        <v>2.5573650008493503</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -15036,11 +15036,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9077868852459015E-5</v>
+        <v>1.8532786885245898E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0244734997409405E-5</v>
+        <v>1.0976501782938649E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15060,55 +15060,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7296319398636704E-2</v>
+        <v>1.6109317086965558E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33950753679986401</v>
+        <v>0.36375807514271147</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86398946716443847</v>
+        <v>0.81316655733123622</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1914797101818391</v>
+        <v>1.0893528778805384</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2141155056533173</v>
+        <v>1.3279388343083158</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3525179084477819</v>
+        <v>1.2729580314802651</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2006431502064263</v>
+        <v>1.1082859848059319</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.9134930142771317</v>
+        <v>0.86781836356327502</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.51031868615788523</v>
+        <v>0.51527323650893264</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.11480140278105208</v>
+        <v>0.10605462923582906</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.3136281628162925E-4</v>
+        <v>6.8213647287805807E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2379549791128626E-4</v>
+        <v>1.2624689390952954E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1351833226661785E-5</v>
+        <v>3.3937551430922555E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15137,11 +15137,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7260928961748631E-5</v>
+        <v>1.8896174863387977E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0140196885190942E-5</v>
+        <v>1.0453811221846331E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15161,7 +15161,7 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6448460604585883E-2</v>
+        <v>1.7465891157446869E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15169,47 +15169,47 @@
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.81316655733123622</v>
+        <v>0.80469607235903584</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1687848585593277</v>
+        <v>1.1460900069368165</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3026447612738716</v>
+        <v>1.2647036517222054</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2994779904694373</v>
+        <v>1.2862180109748513</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1544645675061791</v>
+        <v>1.2006431502064263</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.86781836356327502</v>
+        <v>0.87695329370604636</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.50536413580683781</v>
+        <v>0.51527323650893264</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10496128254267618</v>
+        <v>0.10605462923582906</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>6.7510413810611936E-4</v>
+        <v>6.8916880764999678E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2624689390952954E-4</v>
+        <v>1.2379549791128626E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3937551430922555E-5</v>
+        <v>3.1675048002194387E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15238,11 +15238,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8714480874316939E-5</v>
+        <v>1.7987704918032785E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0871963670720186E-5</v>
+        <v>1.0767425558501721E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -15262,55 +15262,55 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6618032363396047E-2</v>
+        <v>1.7465891157446869E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35336498728149113</v>
+        <v>0.35682934990189791</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.82163704230343659</v>
+        <v>0.88093043710883923</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1801322843705835</v>
+        <v>1.1460900069368165</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3152917977910936</v>
+        <v>1.2394095786877612</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2729580314802651</v>
+        <v>1.3259979494586096</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1890985045313645</v>
+        <v>1.2006431502064263</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.92262794441990303</v>
+        <v>0.90435808413436036</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.47563683370055321</v>
+        <v>0.50536413580683781</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.10386793584952331</v>
+        <v>0.1137080560878992</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>7.1729814673775183E-4</v>
+        <v>6.8916880764999678E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2869828990777284E-4</v>
+        <v>1.2379549791128626E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.1351833226661785E-5</v>
+        <v>3.1028618451129191E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Winter'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -17001,7 +17001,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26461,11 +26461,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5380327868852458E-5</v>
+        <v>5.941847677595628E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.2270915241839627E-5</v>
+        <v>3.3588095455792262E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26485,15 +26485,15 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.232594661952069E-2</v>
+        <v>5.1797401704171998E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1366392708945414</v>
+        <v>1.1475684946531426</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.831571946202494</v>
+        <v>2.5888657793851371</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26501,39 +26501,39 @@
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8774919281274078</v>
+        <v>4.0373885024831777</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.2529393613846489</v>
+        <v>4.0002894983320951</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5390905557484995</v>
+        <v>3.7971492421051609</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8991665542656326</v>
+        <v>2.7843480768689739</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5368989399346158</v>
+        <v>1.5524231716511272</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.36106485772048624</v>
+        <v>0.33329063789583346</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.260982268123028E-3</v>
+        <v>2.2170796998099598E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.797094861479382E-4</v>
+        <v>3.7219048642223642E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.5817020206638006E-5</v>
+        <v>1.0070564368656853E-4</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26558,63 +26558,63 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2457567054416341</v>
+        <v>2.3138099389398654</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.094809981361895</v>
+        <v>1.9352054113533694</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.17246937268107</v>
+        <v>2.0889128583471828</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9520689695862938</v>
+        <v>2.072815503787508</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7407175937663342</v>
+        <v>1.6874303204877728</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5224512142938278</v>
+        <v>1.6017455483716314</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.355487606102185</v>
+        <v>1.4839022214171291</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3058405280750971</v>
+        <v>1.2546310956015636</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2206190761084481</v>
+        <v>1.2087684054666183</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.111195093805877</v>
+        <v>1.0567247460702947</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0871727552492589</v>
+        <v>1.0649855561625392</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1035633100655355</v>
+        <v>1.0178496549148142</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.94919901747301971</v>
+        <v>1.0191399977078739</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0127904814428692</v>
+        <v>0.97227886218515425</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2560993014123187</v>
+        <v>1.2187894211723487</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26622,19 +26622,19 @@
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3761630809649468</v>
+        <v>1.4463754830549949</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5226698995070955</v>
+        <v>1.665420202585886</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5239694230059164</v>
+        <v>1.5843246476794182</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115891939648149</v>
+        <v>1.5745720770466822</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -26642,15 +26642,15 @@
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6626941261406909</v>
+        <v>1.7130787966298029</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6131555114986291</v>
+        <v>1.5966947409731327</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7700723518498298</v>
+        <v>1.9563957573077071</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -26663,11 +26663,11 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3305887978142075E-5</v>
+        <v>2.422889344262295E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2776648075340586E-5</v>
+        <v>1.3830392246502697E-5</v>
       </c>
       <c r="E5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26691,39 +26691,39 @@
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.42842557133717324</v>
+        <v>0.41968219233029214</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0894810154912453</v>
+        <v>1.1218418377335595</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4243568924129162</v>
+        <v>1.3807541304002759</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.614955400993271</v>
+        <v>1.5829760861221172</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.684332420350356</v>
+        <v>1.6674890961468525</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4746210648952083</v>
+        <v>1.4598748542462563</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0907755352682578</v>
+        <v>1.1826303171855848</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63959834672026439</v>
+        <v>0.61475957597384634</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14164852110572923</v>
+        <v>0.13192754416710076</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26731,11 +26731,11 @@
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5338759440431562E-4</v>
+        <v>1.4436479473347352E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9891167596232968E-5</v>
+        <v>3.8326808082655205E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26764,11 +26764,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2152131147540982E-5</v>
+        <v>2.422889344262295E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3830392246502697E-5</v>
+        <v>1.3698674225107434E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26788,27 +26788,27 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2198886444645145E-2</v>
+        <v>2.1141796613947755E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44154063984749486</v>
+        <v>0.41531050282685161</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1218418377335595</v>
+        <v>1.0894810154912453</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4679596544255566</v>
+        <v>1.3807541304002759</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.614955400993271</v>
+        <v>1.6309450584288481</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7180190687573631</v>
+        <v>1.6169591235363416</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26816,15 +26816,15 @@
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.159666621706253</v>
+        <v>1.2055940126649165</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62717896134705542</v>
+        <v>0.61475957597384634</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14025981011449659</v>
+        <v>0.14164852110572923</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26832,11 +26832,11 @@
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5338759440431562E-4</v>
+        <v>1.4586859467861387E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9108987839444087E-5</v>
+        <v>4.1064437231416293E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26865,11 +26865,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2382882513661202E-5</v>
+        <v>2.3075136612021857E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2776648075340586E-5</v>
+        <v>1.2644930053945321E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26889,15 +26889,15 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.156463254622671E-2</v>
+        <v>2.1353214580087234E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.44154063984749486</v>
+        <v>0.43279726084061382</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0355463117540549</v>
+        <v>1.0786940747438072</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26905,27 +26905,27 @@
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6309450584288481</v>
+        <v>1.5989657435576941</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6338024477398454</v>
+        <v>1.684332420350356</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4008900116504479</v>
+        <v>1.4451286435973041</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1252210784872554</v>
+        <v>1.1826303171855848</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.61475957597384634</v>
+        <v>0.62096926866045088</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14164852110572923</v>
+        <v>0.14581465407942715</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -26933,11 +26933,11 @@
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5338759440431562E-4</v>
+        <v>1.5789899423973667E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.715353844747188E-5</v>
+        <v>4.0282257474627412E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27220,7 +27220,7 @@
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4246685562768586E-5</v>
+        <v>3.4575980616256741E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27240,11 +27240,11 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.1797401704171998E-2</v>
+        <v>5.4968671196264161E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1257100471359398</v>
+        <v>1.1147808233773386</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27252,35 +27252,35 @@
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.4518853260006899</v>
+        <v>3.7425704060849583</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9174660717163503</v>
+        <v>3.8375177845384654</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0002894983320951</v>
+        <v>4.168722740367131</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5759560823708805</v>
+        <v>3.6128216089932601</v>
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7269388381706445</v>
+        <v>3.0139850316622914</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.58347163508415</v>
+        <v>1.5524231716511272</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.35064952528624149</v>
+        <v>0.35759308024240466</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.2170796998099598E-3</v>
+        <v>2.260982268123028E-3</v>
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27288,7 +27288,7 @@
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.6794744902624103E-5</v>
+        <v>1.0168336838255463E-4</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27313,59 +27313,59 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.223072294275557</v>
+        <v>2.1550190607773256</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9352054113533694</v>
+        <v>2.0150076963576322</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.068023729763711</v>
+        <v>2.0471346011802392</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9520689695862938</v>
+        <v>1.9721933919531629</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8472921403234566</v>
+        <v>1.7407175937663342</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6651810156338742</v>
+        <v>1.5383100811093886</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4696339308265798</v>
+        <v>1.4839022214171291</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2290263793647971</v>
+        <v>1.2162240212464137</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.2087684054666183</v>
+        <v>1.1495150522574702</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1329832329001097</v>
+        <v>1.0785128851645276</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0538919566191796</v>
+        <v>1.1426407529660578</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0607064824901749</v>
+        <v>1.0285638618086543</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0091484291028947</v>
+        <v>0.99915686049791552</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0127904814428692</v>
+        <v>1.0026625766284405</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -27373,39 +27373,39 @@
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4507570978980424</v>
+        <v>1.3391603980597313</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4604179634730046</v>
+        <v>1.4182905222189757</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5385310442936277</v>
+        <v>1.5543921890801602</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.508880616837541</v>
+        <v>1.5239694230059164</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4958434731943482</v>
+        <v>1.590317797817149</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.797920538892894</v>
+        <v>1.6941943539567657</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6794890163037282</v>
+        <v>1.6626941261406909</v>
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.678998593600614</v>
+        <v>1.5966947409731327</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8259693734871931</v>
+        <v>1.8818663951245562</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -27418,7 +27418,7 @@
       </c>
       <c r="C5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3536639344262295E-5</v>
+        <v>2.3305887978142075E-5</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27442,11 +27442,11 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.050754271552932E-2</v>
+        <v>2.156463254622671E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43279726084061382</v>
+        <v>0.41531050282685161</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27454,15 +27454,15 @@
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5115624164381969</v>
+        <v>1.4824939084297701</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5509967712509631</v>
+        <v>1.6789140307355788</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7517057171643704</v>
+        <v>1.7180190687573631</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27470,27 +27470,27 @@
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1941121649252506</v>
+        <v>1.1711484694459189</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.60234019060063737</v>
+        <v>0.61475957597384634</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14581465407942715</v>
+        <v>0.13609367714079867</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4292931161091531E-4</v>
+        <v>8.7805136626137011E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5489139434945597E-4</v>
+        <v>1.5338759440431562E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0282257474627412E-5</v>
+        <v>4.0673347353021849E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27523,7 +27523,7 @@
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3698674225107434E-5</v>
+        <v>1.2644930053945321E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27543,55 +27543,55 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1776050512366189E-2</v>
+        <v>2.1353214580087234E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45902739786125707</v>
+        <v>0.41531050282685161</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1110548969861214</v>
+        <v>1.0355463117540549</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3807541304002759</v>
+        <v>1.4243568924129162</v>
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5829760861221172</v>
+        <v>1.5509967712509631</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6001157993328381</v>
+        <v>1.6169591235363416</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5336059074910167</v>
+        <v>1.4598748542462563</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1826303171855848</v>
+        <v>1.159666621706253</v>
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63338865403365996</v>
+        <v>0.60234019060063737</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.14581465407942715</v>
+        <v>0.13192754416710076</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.8683187992398386E-4</v>
+        <v>9.2195393457443866E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5037999451403492E-4</v>
+        <v>1.5188379445917527E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7935718204260761E-5</v>
+        <v>3.8326808082655205E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27620,7 +27620,7 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3075136612021857E-5</v>
+        <v>2.2152131147540982E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27644,43 +27644,43 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.156463254622671E-2</v>
+        <v>2.1141796613947755E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43279726084061382</v>
+        <v>0.44591232935093544</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1002679562386835</v>
+        <v>1.046333252501493</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4098226384087029</v>
+        <v>1.4243568924129162</v>
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.56698642868654</v>
+        <v>1.5989657435576941</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6338024477398454</v>
+        <v>1.7685490413678739</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4303824329483521</v>
+        <v>1.5188596968420645</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0907755352682578</v>
+        <v>1.2055940126649165</v>
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.65201773209347347</v>
+        <v>0.59613049791403283</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13887109912326395</v>
+        <v>0.14442594308819451</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27688,11 +27688,11 @@
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4887619456889457E-4</v>
+        <v>1.4586859467861387E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.1064437231416293E-5</v>
+        <v>3.715353844747188E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27890,11 +27890,11 @@
       </c>
       <c r="C3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.5957206284153008E-5</v>
+        <v>5.6534084699453551E-5</v>
       </c>
       <c r="D3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.3258800402304106E-5</v>
+        <v>3.1941620188351465E-5</v>
       </c>
       <c r="E3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27914,27 +27914,27 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>5.0740311873474608E-2</v>
+        <v>5.549721611161286E-2</v>
       </c>
       <c r="J3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0710639283429331</v>
+        <v>1.0929223758601359</v>
       </c>
       <c r="K3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.7237025387281131</v>
+        <v>2.6697678349909229</v>
       </c>
       <c r="L3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.633563501053358</v>
+        <v>3.7789060410954924</v>
       </c>
       <c r="M3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9174660717163503</v>
+        <v>4.1573109332500042</v>
       </c>
       <c r="N3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>4.0423978088408541</v>
+        <v>4.2108310508758899</v>
       </c>
       <c r="O3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27942,15 +27942,15 @@
       </c>
       <c r="P3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.8704619349164679</v>
+        <v>2.7556434575198092</v>
       </c>
       <c r="Q3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.598995866800661</v>
+        <v>1.5368989399346158</v>
       </c>
       <c r="R3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.33329063789583346</v>
+        <v>0.36453663519856788</v>
       </c>
       <c r="S3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27958,11 +27958,11 @@
       </c>
       <c r="T3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.5715248697083292E-4</v>
+        <v>3.6091198683368378E-4</v>
       </c>
       <c r="U3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.483929551065191E-5</v>
+        <v>9.5817020206638006E-5</v>
       </c>
       <c r="V3" s="7">
         <f ca="1">VLOOKUP($A3,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -27987,87 +27987,87 @@
       </c>
       <c r="B4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!B$5:B$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1550190607773256</v>
+        <v>2.3364943501059425</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$5:C$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9352054113533694</v>
+        <v>2.0549088388597636</v>
       </c>
       <c r="D4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$5:D$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1933585012645422</v>
+        <v>2.17246937268107</v>
       </c>
       <c r="E4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$5:E$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0124422366869013</v>
+        <v>2.1130643485212461</v>
       </c>
       <c r="F4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!F$5:F$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.8295297158972694</v>
+        <v>1.7940048670448951</v>
       </c>
       <c r="G4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!G$5:G$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5065923474782672</v>
+        <v>1.5383100811093886</v>
       </c>
       <c r="H4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!H$5:H$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3697558966927346</v>
+        <v>1.4696339308265798</v>
       </c>
       <c r="I4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$5:I$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.31864288619348</v>
+        <v>1.3058405280750971</v>
       </c>
       <c r="J4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$5:J$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.185067064182959</v>
+        <v>1.1258137109738111</v>
       </c>
       <c r="K4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$5:K$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1003010242587605</v>
+        <v>1.0785128851645276</v>
       </c>
       <c r="L4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$5:L$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0871727552492589</v>
+        <v>1.0649855561625392</v>
       </c>
       <c r="M4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$5:M$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1142775169593757</v>
+        <v>1.1249917238532159</v>
       </c>
       <c r="N4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$5:N$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.96918215468297808</v>
+        <v>1.0491147035228112</v>
       </c>
       <c r="O4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$5:O$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0533021007005841</v>
+        <v>0.98240676699958296</v>
       </c>
       <c r="P4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$5:P$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1814795409323788</v>
+        <v>1.243662674665662</v>
       </c>
       <c r="Q4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$5:Q$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3531099855395203</v>
+        <v>1.3252108105799425</v>
       </c>
       <c r="R4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$5:R$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4463754830549949</v>
+        <v>1.3480781201289271</v>
       </c>
       <c r="S4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$5:S$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6336979130128215</v>
+        <v>1.5543921890801602</v>
       </c>
       <c r="T4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$5:T$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4334365859956639</v>
+        <v>1.508880616837541</v>
       </c>
       <c r="U4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$5:U$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5273349147352819</v>
+        <v>1.4958434731943482</v>
       </c>
       <c r="V4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$5:V$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6596189589780561</v>
+        <v>1.6423312614887011</v>
       </c>
       <c r="W4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!W$5:W$7)*(RANDBETWEEN(95,105)/100))</f>
@@ -28075,11 +28075,11 @@
       </c>
       <c r="X4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!X$5:X$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7283809051771026</v>
+        <v>1.678998593600614</v>
       </c>
       <c r="Y4" s="9">
         <f ca="1">VLOOKUP($A4,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Y$5:Y$7)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.9377634167619193</v>
+        <v>1.7700723518498298</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -28116,55 +28116,55 @@
       </c>
       <c r="I5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.050754271552932E-2</v>
+        <v>2.1987468478505665E-2</v>
       </c>
       <c r="J5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43279726084061382</v>
+        <v>0.45465570835781655</v>
       </c>
       <c r="K5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.046333252501493</v>
+        <v>1.0786940747438072</v>
       </c>
       <c r="L5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3952883844044894</v>
+        <v>1.4824939084297701</v>
       </c>
       <c r="M5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5989657435576941</v>
+        <v>1.5509967712509631</v>
       </c>
       <c r="N5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6169591235363416</v>
+        <v>1.6506457719433489</v>
       </c>
       <c r="O5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5483521181399686</v>
+        <v>1.5336059074910167</v>
       </c>
       <c r="P5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1252210784872554</v>
+        <v>1.2055940126649165</v>
       </c>
       <c r="Q5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62717896134705542</v>
+        <v>0.61475957597384634</v>
       </c>
       <c r="R5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.1333162551583334</v>
+        <v>0.13609367714079867</v>
       </c>
       <c r="S5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.4292931161091531E-4</v>
+        <v>8.6927085259875636E-4</v>
       </c>
       <c r="T5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5338759440431562E-4</v>
+        <v>1.5188379445917527E-4</v>
       </c>
       <c r="U5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.8326808082655205E-5</v>
+        <v>3.9500077717838531E-5</v>
       </c>
       <c r="V5" s="7">
         <f ca="1">VLOOKUP($A5,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28193,11 +28193,11 @@
       </c>
       <c r="C6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3305887978142075E-5</v>
+        <v>2.2382882513661202E-5</v>
       </c>
       <c r="D6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.290836609673585E-5</v>
+        <v>1.3830392246502697E-5</v>
       </c>
       <c r="E6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28217,15 +28217,15 @@
       </c>
       <c r="I6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.0930378647808275E-2</v>
+        <v>2.1776050512366189E-2</v>
       </c>
       <c r="J6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.43716895034405434</v>
+        <v>0.42842557133717324</v>
       </c>
       <c r="K6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.0571201932489309</v>
+        <v>1.1110548969861214</v>
       </c>
       <c r="L6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28233,15 +28233,15 @@
       </c>
       <c r="M6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5989657435576941</v>
+        <v>1.614955400993271</v>
       </c>
       <c r="N6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.7517057171643704</v>
+        <v>1.6001157993328381</v>
       </c>
       <c r="O6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5336059074910167</v>
+        <v>1.5188596968420645</v>
       </c>
       <c r="P6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28249,23 +28249,23 @@
       </c>
       <c r="Q6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.62717896134705542</v>
+        <v>0.63959834672026439</v>
       </c>
       <c r="R6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13609367714079867</v>
+        <v>0.14164852110572923</v>
       </c>
       <c r="S6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>8.9561239358659751E-4</v>
+        <v>8.6049033893614271E-4</v>
       </c>
       <c r="T6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5789899423973667E-4</v>
+        <v>1.5338759440431562E-4</v>
       </c>
       <c r="U6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.9891167596232968E-5</v>
+        <v>3.8326808082655205E-5</v>
       </c>
       <c r="V6" s="7">
         <f ca="1">VLOOKUP($A6,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28294,11 +28294,11 @@
       </c>
       <c r="C7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!C$2:C$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.3998142076502733E-5</v>
+        <v>2.2382882513661202E-5</v>
       </c>
       <c r="D7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!D$2:D$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.3040084118131113E-5</v>
+        <v>1.2513212032550058E-5</v>
       </c>
       <c r="E7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!E$2:E$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28318,15 +28318,15 @@
       </c>
       <c r="I7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!I$2:I$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>2.1776050512366189E-2</v>
+        <v>2.2198886444645145E-2</v>
       </c>
       <c r="J7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!J$2:J$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.45902739786125707</v>
+        <v>0.44591232935093544</v>
       </c>
       <c r="K7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!K$2:K$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.1218418377335595</v>
+        <v>1.0247593710066167</v>
       </c>
       <c r="L7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!L$2:L$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28334,15 +28334,15 @@
       </c>
       <c r="M7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!M$2:M$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.5190174563798093</v>
+        <v>1.56698642868654</v>
       </c>
       <c r="N7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!N$2:N$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.6338024477398454</v>
+        <v>1.7517057171643704</v>
       </c>
       <c r="O7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!O$2:O$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4156362222993999</v>
+        <v>1.4303824329483521</v>
       </c>
       <c r="P7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!P$2:P$4)*(RANDBETWEEN(95,105)/100))</f>
@@ -28350,23 +28350,23 @@
       </c>
       <c r="Q7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!Q$2:Q$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.63338865403365996</v>
+        <v>0.63959834672026439</v>
       </c>
       <c r="R7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!R$2:R$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>0.13748238813203131</v>
+        <v>0.14164852110572923</v>
       </c>
       <c r="S7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!S$2:S$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>9.2195393457443866E-4</v>
+        <v>8.7805136626137011E-4</v>
       </c>
       <c r="T7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!T$2:T$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>1.4436479473347352E-4</v>
+        <v>1.5037999451403492E-4</v>
       </c>
       <c r="U7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!U$2:U$4)*(RANDBETWEEN(95,105)/100))</f>
-        <v>3.7544628325866324E-5</v>
+        <v>4.0282257474627412E-5</v>
       </c>
       <c r="V7" s="7">
         <f ca="1">VLOOKUP($A7,'RES installed'!$A$2:$C$6,3,FALSE)*(AVERAGE('[1]Profiles, RES, Summer'!V$2:V$4)*(RANDBETWEEN(95,105)/100))</f>

</xml_diff>